<commit_message>
Date array index values fixed.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvrthotapalli\OneDrive - Computer Generated Solutions, Inc\Documents\UiPath\CGS_HYD_eSSL Logs Update_Linear Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgsinc1-my.sharepoint.com/personal/hvrthotapalli_cgsinc_com/Documents/Documents/UiPath/CGSHYD_HReSSL-main/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF98500-BA62-461C-B322-223DA27B7044}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>